<commit_message>
Slices, transforms and autorotations complete
</commit_message>
<xml_diff>
--- a/_docs/Patron.xlsx
+++ b/_docs/Patron.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\redes\_docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{579C10D5-ED57-4A31-AB10-892263AFEC24}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D34435A9-2429-4399-8D22-BDF9E202CD84}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="450" windowWidth="28800" windowHeight="12360" xr2:uid="{336DEFCC-A4AB-4BC7-97E8-3FC4688F9665}"/>
+    <workbookView xWindow="0" yWindow="900" windowWidth="28800" windowHeight="12360" xr2:uid="{336DEFCC-A4AB-4BC7-97E8-3FC4688F9665}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -170,13 +170,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -191,14 +185,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -516,66 +516,66 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B7461CC-2B5D-4E79-9948-26ED26294D91}">
   <dimension ref="A1:K32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6:K32"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6:H32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="3.7109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="3" style="3" customWidth="1"/>
-    <col min="3" max="11" width="6.28515625" style="3" customWidth="1"/>
-    <col min="12" max="16384" width="11.42578125" style="3"/>
+    <col min="1" max="1" width="3.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="3" style="2" customWidth="1"/>
+    <col min="3" max="11" width="6.28515625" style="2" customWidth="1"/>
+    <col min="12" max="16384" width="11.42578125" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B1" s="7"/>
-      <c r="C1" s="4" t="s">
+      <c r="B1" s="5"/>
+      <c r="C1" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4"/>
-      <c r="H1" s="4"/>
-      <c r="I1" s="4"/>
-      <c r="J1" s="4"/>
-      <c r="K1" s="4"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
+      <c r="G1" s="10"/>
+      <c r="H1" s="10"/>
+      <c r="I1" s="10"/>
+      <c r="J1" s="10"/>
+      <c r="K1" s="10"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B2" s="7"/>
-      <c r="C2" s="2">
+      <c r="B2" s="5"/>
+      <c r="C2" s="9">
         <v>3</v>
       </c>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2">
+      <c r="D2" s="9"/>
+      <c r="E2" s="9"/>
+      <c r="F2" s="9">
         <v>2</v>
       </c>
-      <c r="G2" s="2"/>
-      <c r="H2" s="2"/>
-      <c r="I2" s="2">
-        <v>1</v>
-      </c>
-      <c r="J2" s="2"/>
-      <c r="K2" s="2"/>
+      <c r="G2" s="9"/>
+      <c r="H2" s="9"/>
+      <c r="I2" s="9">
+        <v>1</v>
+      </c>
+      <c r="J2" s="9"/>
+      <c r="K2" s="9"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B3" s="7"/>
-      <c r="C3" s="4" t="s">
+      <c r="B3" s="5"/>
+      <c r="C3" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="4"/>
-      <c r="E3" s="4"/>
-      <c r="F3" s="4"/>
-      <c r="G3" s="4"/>
-      <c r="H3" s="4"/>
-      <c r="I3" s="4"/>
-      <c r="J3" s="4"/>
-      <c r="K3" s="4"/>
+      <c r="D3" s="10"/>
+      <c r="E3" s="10"/>
+      <c r="F3" s="10"/>
+      <c r="G3" s="10"/>
+      <c r="H3" s="10"/>
+      <c r="I3" s="10"/>
+      <c r="J3" s="10"/>
+      <c r="K3" s="10"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B4" s="7"/>
+      <c r="B4" s="5"/>
       <c r="C4" s="1">
         <v>1</v>
       </c>
@@ -605,37 +605,37 @@
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B5" s="8"/>
-      <c r="C5" s="5" t="s">
+      <c r="B5" s="6"/>
+      <c r="C5" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="D5" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="E5" s="5" t="s">
+      <c r="D5" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E5" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="F5" s="5" t="s">
+      <c r="F5" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="G5" s="5" t="s">
+      <c r="G5" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="H5" s="5" t="s">
+      <c r="H5" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="I5" s="5" t="s">
+      <c r="I5" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="J5" s="5" t="s">
+      <c r="J5" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="K5" s="5" t="s">
+      <c r="K5" s="3" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" s="9" t="s">
+      <c r="A6" s="11" t="s">
         <v>11</v>
       </c>
       <c r="B6" s="1">
@@ -651,14 +651,14 @@
       </c>
       <c r="G6" s="1"/>
       <c r="H6" s="1"/>
-      <c r="I6" s="6">
+      <c r="I6" s="4">
         <v>1</v>
       </c>
       <c r="J6" s="1"/>
       <c r="K6" s="1"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" s="9"/>
+      <c r="A7" s="11"/>
       <c r="B7" s="1">
         <v>2</v>
       </c>
@@ -679,7 +679,7 @@
       <c r="K7" s="1"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" s="9"/>
+      <c r="A8" s="11"/>
       <c r="B8" s="1">
         <v>3</v>
       </c>
@@ -700,7 +700,7 @@
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" s="9"/>
+      <c r="A9" s="11"/>
       <c r="B9" s="1">
         <v>4</v>
       </c>
@@ -714,14 +714,14 @@
       </c>
       <c r="G9" s="1"/>
       <c r="H9" s="1"/>
-      <c r="I9" s="6">
+      <c r="I9" s="4">
         <v>1</v>
       </c>
       <c r="J9" s="1"/>
       <c r="K9" s="1"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="9"/>
+      <c r="A10" s="11"/>
       <c r="B10" s="1">
         <v>5</v>
       </c>
@@ -742,7 +742,7 @@
       <c r="K10" s="1"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" s="9"/>
+      <c r="A11" s="11"/>
       <c r="B11" s="1">
         <v>6</v>
       </c>
@@ -763,7 +763,7 @@
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" s="9"/>
+      <c r="A12" s="11"/>
       <c r="B12" s="1">
         <v>7</v>
       </c>
@@ -777,14 +777,14 @@
       </c>
       <c r="G12" s="1"/>
       <c r="H12" s="1"/>
-      <c r="I12" s="6">
+      <c r="I12" s="4">
         <v>1</v>
       </c>
       <c r="J12" s="1"/>
       <c r="K12" s="1"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13" s="9"/>
+      <c r="A13" s="11"/>
       <c r="B13" s="1">
         <v>8</v>
       </c>
@@ -805,7 +805,7 @@
       <c r="K13" s="1"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A14" s="9"/>
+      <c r="A14" s="11"/>
       <c r="B14" s="1">
         <v>9</v>
       </c>
@@ -826,7 +826,7 @@
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A15" s="9"/>
+      <c r="A15" s="11"/>
       <c r="B15" s="1">
         <v>10</v>
       </c>
@@ -840,14 +840,14 @@
         <v>1</v>
       </c>
       <c r="H15" s="1"/>
-      <c r="I15" s="6">
+      <c r="I15" s="4">
         <v>1</v>
       </c>
       <c r="J15" s="1"/>
       <c r="K15" s="1"/>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A16" s="9"/>
+      <c r="A16" s="11"/>
       <c r="B16" s="1">
         <v>11</v>
       </c>
@@ -868,7 +868,7 @@
       <c r="K16" s="1"/>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A17" s="9"/>
+      <c r="A17" s="11"/>
       <c r="B17" s="1">
         <v>12</v>
       </c>
@@ -889,7 +889,7 @@
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A18" s="9"/>
+      <c r="A18" s="11"/>
       <c r="B18" s="1">
         <v>13</v>
       </c>
@@ -903,14 +903,14 @@
         <v>1</v>
       </c>
       <c r="H18" s="1"/>
-      <c r="I18" s="6">
+      <c r="I18" s="4">
         <v>1</v>
       </c>
       <c r="J18" s="1"/>
       <c r="K18" s="1"/>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A19" s="9"/>
+      <c r="A19" s="11"/>
       <c r="B19" s="1">
         <v>14</v>
       </c>
@@ -931,7 +931,7 @@
       <c r="K19" s="1"/>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A20" s="9"/>
+      <c r="A20" s="11"/>
       <c r="B20" s="1">
         <v>15</v>
       </c>
@@ -952,7 +952,7 @@
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A21" s="9"/>
+      <c r="A21" s="11"/>
       <c r="B21" s="1">
         <v>16</v>
       </c>
@@ -966,14 +966,14 @@
         <v>1</v>
       </c>
       <c r="H21" s="1"/>
-      <c r="I21" s="6">
+      <c r="I21" s="4">
         <v>1</v>
       </c>
       <c r="J21" s="1"/>
       <c r="K21" s="1"/>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A22" s="9"/>
+      <c r="A22" s="11"/>
       <c r="B22" s="1">
         <v>17</v>
       </c>
@@ -994,7 +994,7 @@
       <c r="K22" s="1"/>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A23" s="9"/>
+      <c r="A23" s="11"/>
       <c r="B23" s="1">
         <v>18</v>
       </c>
@@ -1015,7 +1015,7 @@
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A24" s="9"/>
+      <c r="A24" s="11"/>
       <c r="B24" s="1">
         <v>19</v>
       </c>
@@ -1029,14 +1029,14 @@
       <c r="H24" s="1">
         <v>1</v>
       </c>
-      <c r="I24" s="6">
+      <c r="I24" s="4">
         <v>1</v>
       </c>
       <c r="J24" s="1"/>
       <c r="K24" s="1"/>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A25" s="9"/>
+      <c r="A25" s="11"/>
       <c r="B25" s="1">
         <v>20</v>
       </c>
@@ -1057,7 +1057,7 @@
       <c r="K25" s="1"/>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A26" s="9"/>
+      <c r="A26" s="11"/>
       <c r="B26" s="1">
         <v>21</v>
       </c>
@@ -1078,7 +1078,7 @@
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A27" s="9"/>
+      <c r="A27" s="11"/>
       <c r="B27" s="1">
         <v>22</v>
       </c>
@@ -1092,14 +1092,14 @@
       <c r="H27" s="1">
         <v>1</v>
       </c>
-      <c r="I27" s="6">
+      <c r="I27" s="4">
         <v>1</v>
       </c>
       <c r="J27" s="1"/>
       <c r="K27" s="1"/>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A28" s="9"/>
+      <c r="A28" s="11"/>
       <c r="B28" s="1">
         <v>23</v>
       </c>
@@ -1120,7 +1120,7 @@
       <c r="K28" s="1"/>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A29" s="9"/>
+      <c r="A29" s="11"/>
       <c r="B29" s="1">
         <v>24</v>
       </c>
@@ -1141,7 +1141,7 @@
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A30" s="9"/>
+      <c r="A30" s="11"/>
       <c r="B30" s="1">
         <v>25</v>
       </c>
@@ -1155,14 +1155,14 @@
       <c r="H30" s="1">
         <v>1</v>
       </c>
-      <c r="I30" s="10">
-        <v>1</v>
-      </c>
-      <c r="J30" s="11"/>
-      <c r="K30" s="11"/>
+      <c r="I30" s="7">
+        <v>1</v>
+      </c>
+      <c r="J30" s="8"/>
+      <c r="K30" s="8"/>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A31" s="9"/>
+      <c r="A31" s="11"/>
       <c r="B31" s="1">
         <v>26</v>
       </c>
@@ -1176,14 +1176,14 @@
       <c r="H31" s="1">
         <v>1</v>
       </c>
-      <c r="I31" s="11"/>
-      <c r="J31" s="11">
-        <v>1</v>
-      </c>
-      <c r="K31" s="11"/>
+      <c r="I31" s="8"/>
+      <c r="J31" s="8">
+        <v>1</v>
+      </c>
+      <c r="K31" s="8"/>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A32" s="9"/>
+      <c r="A32" s="11"/>
       <c r="B32" s="1">
         <v>27</v>
       </c>
@@ -1197,20 +1197,20 @@
       <c r="H32" s="1">
         <v>1</v>
       </c>
-      <c r="I32" s="11"/>
-      <c r="J32" s="11"/>
-      <c r="K32" s="11">
+      <c r="I32" s="8"/>
+      <c r="J32" s="8"/>
+      <c r="K32" s="8">
         <v>1</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="6">
+    <mergeCell ref="A6:A32"/>
     <mergeCell ref="C2:E2"/>
     <mergeCell ref="F2:H2"/>
     <mergeCell ref="I2:K2"/>
     <mergeCell ref="C1:K1"/>
     <mergeCell ref="C3:K3"/>
-    <mergeCell ref="A6:A32"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
fixed spelling issues in images, added conclusions to data.db
</commit_message>
<xml_diff>
--- a/_docs/Patron.xlsx
+++ b/_docs/Patron.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\redes\_docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Documentos\dev\redesCube\_docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D34435A9-2429-4399-8D22-BDF9E202CD84}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A2FC0C3-0FFC-45C4-B9C1-E4FFF947891D}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="900" windowWidth="28800" windowHeight="12360" xr2:uid="{336DEFCC-A4AB-4BC7-97E8-3FC4688F9665}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -191,14 +191,14 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -218,7 +218,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -517,10 +517,10 @@
   <dimension ref="A1:K32"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6:H32"/>
+      <selection activeCell="B29" sqref="A29:XFD29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3.7109375" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="3" style="2" customWidth="1"/>
@@ -530,49 +530,49 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B1" s="5"/>
-      <c r="C1" s="10" t="s">
+      <c r="C1" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10"/>
-      <c r="F1" s="10"/>
-      <c r="G1" s="10"/>
-      <c r="H1" s="10"/>
-      <c r="I1" s="10"/>
-      <c r="J1" s="10"/>
-      <c r="K1" s="10"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
+      <c r="G1" s="11"/>
+      <c r="H1" s="11"/>
+      <c r="I1" s="11"/>
+      <c r="J1" s="11"/>
+      <c r="K1" s="11"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B2" s="5"/>
-      <c r="C2" s="9">
+      <c r="C2" s="10">
         <v>3</v>
       </c>
-      <c r="D2" s="9"/>
-      <c r="E2" s="9"/>
-      <c r="F2" s="9">
+      <c r="D2" s="10"/>
+      <c r="E2" s="10"/>
+      <c r="F2" s="10">
         <v>2</v>
       </c>
-      <c r="G2" s="9"/>
-      <c r="H2" s="9"/>
-      <c r="I2" s="9">
-        <v>1</v>
-      </c>
-      <c r="J2" s="9"/>
-      <c r="K2" s="9"/>
+      <c r="G2" s="10"/>
+      <c r="H2" s="10"/>
+      <c r="I2" s="10">
+        <v>1</v>
+      </c>
+      <c r="J2" s="10"/>
+      <c r="K2" s="10"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B3" s="5"/>
-      <c r="C3" s="10" t="s">
+      <c r="C3" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="10"/>
-      <c r="E3" s="10"/>
-      <c r="F3" s="10"/>
-      <c r="G3" s="10"/>
-      <c r="H3" s="10"/>
-      <c r="I3" s="10"/>
-      <c r="J3" s="10"/>
-      <c r="K3" s="10"/>
+      <c r="D3" s="11"/>
+      <c r="E3" s="11"/>
+      <c r="F3" s="11"/>
+      <c r="G3" s="11"/>
+      <c r="H3" s="11"/>
+      <c r="I3" s="11"/>
+      <c r="J3" s="11"/>
+      <c r="K3" s="11"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B4" s="5"/>
@@ -634,8 +634,8 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" s="11" t="s">
+    <row r="6" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="9" t="s">
         <v>11</v>
       </c>
       <c r="B6" s="1">
@@ -657,8 +657,8 @@
       <c r="J6" s="1"/>
       <c r="K6" s="1"/>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" s="11"/>
+    <row r="7" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="9"/>
       <c r="B7" s="1">
         <v>2</v>
       </c>
@@ -678,8 +678,8 @@
       </c>
       <c r="K7" s="1"/>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" s="11"/>
+    <row r="8" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="9"/>
       <c r="B8" s="1">
         <v>3</v>
       </c>
@@ -699,8 +699,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" s="11"/>
+    <row r="9" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="9"/>
       <c r="B9" s="1">
         <v>4</v>
       </c>
@@ -720,8 +720,8 @@
       <c r="J9" s="1"/>
       <c r="K9" s="1"/>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="11"/>
+    <row r="10" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="9"/>
       <c r="B10" s="1">
         <v>5</v>
       </c>
@@ -741,8 +741,8 @@
       </c>
       <c r="K10" s="1"/>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" s="11"/>
+    <row r="11" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="9"/>
       <c r="B11" s="1">
         <v>6</v>
       </c>
@@ -762,8 +762,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" s="11"/>
+    <row r="12" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="9"/>
       <c r="B12" s="1">
         <v>7</v>
       </c>
@@ -783,8 +783,8 @@
       <c r="J12" s="1"/>
       <c r="K12" s="1"/>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13" s="11"/>
+    <row r="13" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="9"/>
       <c r="B13" s="1">
         <v>8</v>
       </c>
@@ -804,8 +804,8 @@
       </c>
       <c r="K13" s="1"/>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A14" s="11"/>
+    <row r="14" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="9"/>
       <c r="B14" s="1">
         <v>9</v>
       </c>
@@ -825,8 +825,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A15" s="11"/>
+    <row r="15" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="9"/>
       <c r="B15" s="1">
         <v>10</v>
       </c>
@@ -846,8 +846,8 @@
       <c r="J15" s="1"/>
       <c r="K15" s="1"/>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A16" s="11"/>
+    <row r="16" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="9"/>
       <c r="B16" s="1">
         <v>11</v>
       </c>
@@ -867,8 +867,8 @@
       </c>
       <c r="K16" s="1"/>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A17" s="11"/>
+    <row r="17" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="9"/>
       <c r="B17" s="1">
         <v>12</v>
       </c>
@@ -888,8 +888,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A18" s="11"/>
+    <row r="18" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="9"/>
       <c r="B18" s="1">
         <v>13</v>
       </c>
@@ -909,8 +909,8 @@
       <c r="J18" s="1"/>
       <c r="K18" s="1"/>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A19" s="11"/>
+    <row r="19" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="9"/>
       <c r="B19" s="1">
         <v>14</v>
       </c>
@@ -930,8 +930,8 @@
       </c>
       <c r="K19" s="1"/>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A20" s="11"/>
+    <row r="20" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="9"/>
       <c r="B20" s="1">
         <v>15</v>
       </c>
@@ -951,8 +951,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A21" s="11"/>
+    <row r="21" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="9"/>
       <c r="B21" s="1">
         <v>16</v>
       </c>
@@ -972,8 +972,8 @@
       <c r="J21" s="1"/>
       <c r="K21" s="1"/>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A22" s="11"/>
+    <row r="22" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="9"/>
       <c r="B22" s="1">
         <v>17</v>
       </c>
@@ -993,8 +993,8 @@
       </c>
       <c r="K22" s="1"/>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A23" s="11"/>
+    <row r="23" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="9"/>
       <c r="B23" s="1">
         <v>18</v>
       </c>
@@ -1014,8 +1014,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A24" s="11"/>
+    <row r="24" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="9"/>
       <c r="B24" s="1">
         <v>19</v>
       </c>
@@ -1035,8 +1035,8 @@
       <c r="J24" s="1"/>
       <c r="K24" s="1"/>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A25" s="11"/>
+    <row r="25" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="9"/>
       <c r="B25" s="1">
         <v>20</v>
       </c>
@@ -1056,8 +1056,8 @@
       </c>
       <c r="K25" s="1"/>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A26" s="11"/>
+    <row r="26" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="9"/>
       <c r="B26" s="1">
         <v>21</v>
       </c>
@@ -1077,8 +1077,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A27" s="11"/>
+    <row r="27" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="9"/>
       <c r="B27" s="1">
         <v>22</v>
       </c>
@@ -1098,8 +1098,8 @@
       <c r="J27" s="1"/>
       <c r="K27" s="1"/>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A28" s="11"/>
+    <row r="28" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="9"/>
       <c r="B28" s="1">
         <v>23</v>
       </c>
@@ -1119,8 +1119,8 @@
       </c>
       <c r="K28" s="1"/>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A29" s="11"/>
+    <row r="29" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="9"/>
       <c r="B29" s="1">
         <v>24</v>
       </c>
@@ -1141,7 +1141,7 @@
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A30" s="11"/>
+      <c r="A30" s="9"/>
       <c r="B30" s="1">
         <v>25</v>
       </c>
@@ -1162,7 +1162,7 @@
       <c r="K30" s="8"/>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A31" s="11"/>
+      <c r="A31" s="9"/>
       <c r="B31" s="1">
         <v>26</v>
       </c>
@@ -1183,7 +1183,7 @@
       <c r="K31" s="8"/>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A32" s="11"/>
+      <c r="A32" s="9"/>
       <c r="B32" s="1">
         <v>27</v>
       </c>

</xml_diff>